<commit_message>
Continued work on plots
</commit_message>
<xml_diff>
--- a/data/sitenames.xlsx
+++ b/data/sitenames.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://drexel0-my.sharepoint.com/personal/lf649_drexel_edu/Documents/Research/South Philly R21/Analysis/source_apportionment/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://drexel0-my.sharepoint.com/personal/lf649_drexel_edu/Documents/Research/South Philly R21/Papers/Analysis Paper/thriveair_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="8_{5334D5FC-2FEB-FD42-97EF-6E6F49FE5F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B99DD0F9-B4A6-2948-A383-35EC5888F529}"/>
+  <xr:revisionPtr revIDLastSave="204" documentId="8_{5334D5FC-2FEB-FD42-97EF-6E6F49FE5F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3E3F424-7C8B-4038-A29A-0017F28CBEBE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{64F79FF7-AE34-C948-8EC1-A489EB5877E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{64F79FF7-AE34-C948-8EC1-A489EB5877E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$J$1:$J$22</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
   <si>
     <t>Bartram’s Garden</t>
   </si>
@@ -292,6 +295,87 @@
   </si>
   <si>
     <t>31st &amp; Grays Ferry</t>
+  </si>
+  <si>
+    <t>#F8766D</t>
+  </si>
+  <si>
+    <t>#D39200</t>
+  </si>
+  <si>
+    <t>#93AA00</t>
+  </si>
+  <si>
+    <t>#00BA38</t>
+  </si>
+  <si>
+    <t>#00C19F</t>
+  </si>
+  <si>
+    <t>#00B9E3</t>
+  </si>
+  <si>
+    <t>#619CFF</t>
+  </si>
+  <si>
+    <t>#DB72FB</t>
+  </si>
+  <si>
+    <t>#FF61C3</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>site_traffic</t>
+  </si>
+  <si>
+    <t>land_use</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Industrial</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>Industrial/Commercial</t>
+  </si>
+  <si>
+    <t>Institutional</t>
+  </si>
+  <si>
+    <t>Industrial/Commercial/Residential</t>
+  </si>
+  <si>
+    <t>Park</t>
+  </si>
+  <si>
+    <t>Institutional/Residential</t>
+  </si>
+  <si>
+    <t>Commercial/Residential</t>
+  </si>
+  <si>
+    <t>Industrial/Park</t>
+  </si>
+  <si>
+    <t>Industrial/Institutional</t>
+  </si>
+  <si>
+    <t>land_use_short</t>
+  </si>
+  <si>
+    <t>Mixed Use</t>
+  </si>
+  <si>
+    <t>Civic/Institution</t>
   </si>
 </sst>
 </file>
@@ -369,9 +453,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -409,7 +493,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -515,7 +599,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -657,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -665,21 +749,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71F45A3-C6A6-7D49-97EE-03EC6C15B526}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.875" customWidth="1"/>
+    <col min="3" max="3" width="24.875" customWidth="1"/>
+    <col min="4" max="4" width="25.375" customWidth="1"/>
+    <col min="6" max="6" width="23.875" customWidth="1"/>
+    <col min="9" max="9" width="23.375" customWidth="1"/>
+    <col min="10" max="10" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -701,455 +787,658 @@
       <c r="G1" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="H4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="H5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>21</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="H11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="H12" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="H13" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" t="s">
+        <v>104</v>
+      </c>
+      <c r="J13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="D22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" t="s">
-        <v>82</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
+      </c>
+      <c r="G22" t="s">
+        <v>93</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="J1:J22" xr:uid="{B71F45A3-C6A6-7D49-97EE-03EC6C15B526}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G22">
+    <sortCondition ref="E2:E22"/>
+    <sortCondition ref="D2:D22"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1162,12 +1451,12 @@
       <selection activeCell="F9" sqref="F9:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1175,7 +1464,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1183,7 +1472,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1191,7 +1480,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1199,7 +1488,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1207,7 +1496,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1215,7 +1504,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1223,7 +1512,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1231,7 +1520,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>